<commit_message>
Updated model, pulled out ATP and Fd rxns
</commit_message>
<xml_diff>
--- a/Matt_Work/ATP_fluxes.xlsx
+++ b/Matt_Work/ATP_fluxes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="96" windowWidth="11460" windowHeight="9264"/>
+    <workbookView xWindow="96" yWindow="96" windowWidth="11460" windowHeight="9264" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Acetate+CO2+H2" sheetId="1" r:id="rId1"/>
@@ -481,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -636,7 +636,7 @@
         <v>37</v>
       </c>
       <c r="C21" s="1">
-        <v>-961.80277100000001</v>
+        <v>961.80277100000001</v>
       </c>
       <c r="D21" t="s">
         <v>31</v>
@@ -650,7 +650,7 @@
         <v>34</v>
       </c>
       <c r="C22">
-        <v>1000</v>
+        <v>-1000</v>
       </c>
       <c r="D22" t="s">
         <v>32</v>
@@ -666,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21:C22"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32:D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -820,7 +820,7 @@
         <v>37</v>
       </c>
       <c r="C21" s="1">
-        <v>-961.80277100000001</v>
+        <v>961.80277100000001</v>
       </c>
       <c r="D21" t="s">
         <v>31</v>
@@ -834,7 +834,7 @@
         <v>34</v>
       </c>
       <c r="C22">
-        <v>1000</v>
+        <v>-1000</v>
       </c>
       <c r="D22" t="s">
         <v>32</v>

</xml_diff>